<commit_message>
few more test runs
</commit_message>
<xml_diff>
--- a/output/Cavaliers_@_Nets_3-21-2023/Forecast.xlsx
+++ b/output/Cavaliers_@_Nets_3-21-2023/Forecast.xlsx
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10.33695793151855</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>31</v>
+        <v>27.75533866882324</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>16.16401100158691</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>2.293780088424683</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>1.674256324768066</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>5.555194854736328</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17</v>
+        <v>19.31033897399902</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>8.197628974914551</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>9.649618148803711</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17</v>
+        <v>16.25031661987305</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -588,7 +588,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>123</v>
+        <v>117.1874389648438</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>15.86654758453369</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>15.42139530181885</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>8.723228454589844</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21</v>
+        <v>23.49494934082031</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>5.346555709838867</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>8.939894676208496</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>12.07424163818359</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>6.25080394744873</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26</v>
+        <v>24.57846260070801</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>125</v>
+        <v>120.6960754394531</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>

</xml_diff>